<commit_message>
Lots of Active Development
Many changes during active development
</commit_message>
<xml_diff>
--- a/Transmission.xlsx
+++ b/Transmission.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9928C6DA-BF2E-4E8F-A427-D6ABEB6E2991}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD26EF0C-8F7C-463B-83CE-0D1684BE4F04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="-110" windowWidth="18050" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="0" windowWidth="17520" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transmission" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>Names</t>
   </si>
@@ -130,10 +130,25 @@
     <t>First six (early sept)</t>
   </si>
   <si>
-    <t>No Io</t>
-  </si>
-  <si>
     <t>No Io and First six</t>
+  </si>
+  <si>
+    <t>No Io and all nights</t>
+  </si>
+  <si>
+    <t>Last Five</t>
+  </si>
+  <si>
+    <t>Jupiter</t>
+  </si>
+  <si>
+    <t>Moons</t>
+  </si>
+  <si>
+    <t>Trans</t>
+  </si>
+  <si>
+    <t>Abs</t>
   </si>
 </sst>
 </file>
@@ -796,7 +811,7 @@
             <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
@@ -2237,7 +2252,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B14667F8-DBB0-4F95-A6CE-91BC2D82D2A4}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2574,10 +2589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3369,22 +3384,25 @@
         <v>0.23906510389751026</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="L19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B22" s="16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
       <c r="B23" s="9">
         <f>AVERAGE(B3:G3)</f>
         <v>1.3174977434176582</v>
@@ -3397,8 +3415,19 @@
         <f>C23/SQRT(COUNT(B3:G3))*1.96</f>
         <v>7.2655644005097924E-3</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="H23">
+        <f>C29/C23</f>
+        <v>3.4960607834295421</v>
+      </c>
+      <c r="I23">
+        <f>D29/D23</f>
+        <v>3.8297427069870862</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
       <c r="B24" s="9">
         <f>AVERAGE(B4:G7)</f>
         <v>1.3610049848024104</v>
@@ -3411,8 +3440,19 @@
         <f>C24/SQRT(COUNT(B4:G7))*1.96</f>
         <v>1.2244454617635417E-2</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="H24">
+        <f>C30/C24</f>
+        <v>1.2868837257095489</v>
+      </c>
+      <c r="I24">
+        <f>D30/D24</f>
+        <v>1.3604783922106594</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
       <c r="B25">
         <f>B23/B24</f>
         <v>0.96803300364761813</v>
@@ -3431,7 +3471,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
       <c r="B26">
         <f>1-B25</f>
         <v>3.1966996352381871E-2</v>
@@ -3452,156 +3495,281 @@
         <v>-0.17492601892449303</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B28" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="9">
+        <f>AVERAGE(H3:L3)</f>
+        <v>1.3104592236269941</v>
+      </c>
+      <c r="C29">
+        <f>_xlfn.STDEV.P(H3:L3)</f>
+        <v>3.1744455723109716E-2</v>
+      </c>
+      <c r="D29">
+        <f>C29/SQRT(COUNT(H3:L3))*1.96</f>
+        <v>2.7825242274997379E-2</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="9">
+        <f>AVERAGE(H4:L7)</f>
+        <v>1.33126839395956</v>
+      </c>
+      <c r="C30">
+        <f>_xlfn.STDEV.P(H4:L7)</f>
+        <v>3.5042855169028705E-2</v>
+      </c>
+      <c r="D30">
+        <f>C30/SQRT(COUNT(H4:L7))*1.96</f>
+        <v>1.6658315931697015E-2</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31">
+        <f>B29/B30</f>
+        <v>0.98436891431736495</v>
+      </c>
+      <c r="D31">
+        <f>SQRT((D29/B29)^2+(D30/B30)^2)*B31</f>
+        <v>2.4260786684453389E-2</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32">
+        <f>1-B31</f>
+        <v>1.5631085682635049E-2</v>
+      </c>
+      <c r="D32">
+        <f>D31</f>
+        <v>2.4260786684453389E-2</v>
+      </c>
+      <c r="E32" s="6">
+        <v>3.8744399999999998E-2</v>
+      </c>
+      <c r="F32" s="3">
+        <f>B32-E32</f>
+        <v>-2.311331431736495E-2</v>
+      </c>
+      <c r="G32" s="7">
+        <f>F32/E32</f>
+        <v>-0.59655883991918701</v>
+      </c>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B34" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="9">
+        <f>AVERAGE(B3:L3)</f>
+        <v>1.3142984162400835</v>
+      </c>
+      <c r="C35" s="9">
+        <f>_xlfn.STDEV.P(B3:L3)</f>
+        <v>2.2700318153770247E-2</v>
+      </c>
+      <c r="D35">
+        <f>C35/SQRT(COUNT(B3:L3))*1.96</f>
+        <v>1.3415030759817117E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="9">
+        <f>AVERAGE(B5:L7)</f>
+        <v>1.3508395569357092</v>
+      </c>
+      <c r="C36">
+        <f>_xlfn.STDEV.P(B5:L7)</f>
+        <v>3.2283159492326796E-2</v>
+      </c>
+      <c r="D36">
+        <f>C36/SQRT(COUNT(B5:L7))*1.96</f>
+        <v>1.1957849617298327E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <f>B35/B36</f>
+        <v>0.97294931103548898</v>
+      </c>
+      <c r="D37">
+        <f>SQRT((D35/B35)^2+(D36/B36)^2)*B37</f>
+        <v>1.3145384294124207E-2</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <f>1-B37</f>
+        <v>2.7050688964511016E-2</v>
+      </c>
+      <c r="D38">
+        <f>D37</f>
+        <v>1.3145384294124207E-2</v>
+      </c>
+      <c r="E38" s="6">
+        <v>3.8744399999999998E-2</v>
+      </c>
+      <c r="F38" s="3">
+        <f>B38-E38</f>
+        <v>-1.1693711035488982E-2</v>
+      </c>
+      <c r="G38" s="7">
+        <f>F38/E38</f>
+        <v>-0.30181680540901351</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B40" s="16" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B29" s="9">
+      <c r="C40" s="16"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="9">
         <f>B23</f>
         <v>1.3174977434176582</v>
       </c>
-      <c r="C29" s="9">
-        <f t="shared" ref="C29:D29" si="6">C23</f>
+      <c r="C41" s="9">
+        <f>C23</f>
         <v>9.0800640176425234E-3</v>
       </c>
-      <c r="D29" s="9">
-        <f t="shared" si="6"/>
+      <c r="D41" s="9">
+        <f>D23</f>
         <v>7.2655644005097924E-3</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B30" s="9">
-        <f>AVERAGE(B5:L7)</f>
-        <v>1.3508395569357092</v>
-      </c>
-      <c r="C30">
-        <f>_xlfn.STDEV.P(B5:L7)</f>
-        <v>3.2283159492326796E-2</v>
-      </c>
-      <c r="D30">
-        <f>C30/SQRT(COUNT(B5:L7))*1.96</f>
-        <v>1.1957849617298327E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B31">
-        <f>B29/B30</f>
-        <v>0.97531771012563129</v>
-      </c>
-      <c r="D31">
-        <f>SQRT((D29/B29)^2+(D30/B30)^2)*B31</f>
-        <v>1.0171976316846474E-2</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B32">
-        <f>1-B31</f>
-        <v>2.4682289874368712E-2</v>
-      </c>
-      <c r="D32">
-        <f>D31</f>
-        <v>1.0171976316846474E-2</v>
-      </c>
-      <c r="E32" s="6">
-        <v>3.8744399999999998E-2</v>
-      </c>
-      <c r="F32" s="3">
-        <f>B32-E32</f>
-        <v>-1.4062110125631286E-2</v>
-      </c>
-      <c r="G32" s="7">
-        <f>F32/E32</f>
-        <v>-0.36294561602789788</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B34" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="16"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B35" s="9">
-        <f>B29</f>
-        <v>1.3174977434176582</v>
-      </c>
-      <c r="C35" s="9">
-        <f t="shared" ref="C35:D35" si="7">C29</f>
-        <v>9.0800640176425234E-3</v>
-      </c>
-      <c r="D35" s="9">
-        <f t="shared" si="7"/>
-        <v>7.2655644005097924E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B36" s="9">
-        <f>AVERAGE(B5:F7)</f>
-        <v>1.3678357265552266</v>
-      </c>
-      <c r="C36">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="9">
+        <f>AVERAGE(B5:G7)</f>
+        <v>1.3635611235408978</v>
+      </c>
+      <c r="C42">
         <f>_xlfn.STDEV.P(B5:G7)</f>
         <v>2.7113412432066344E-2</v>
       </c>
-      <c r="D36">
-        <f>C36/SQRT(COUNT(B5:F7))*1.96</f>
-        <v>1.60230028194282E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B37">
-        <f>B35/B36</f>
-        <v>0.96319880950591918</v>
-      </c>
-      <c r="D37">
-        <f>SQRT((D35/B35)^2+(D36/B36)^2)*B37</f>
-        <v>1.2470816356674488E-2</v>
-      </c>
-      <c r="E37" s="6" t="s">
+      <c r="D42">
+        <f>C42/SQRT(COUNT(B5:G7))*1.96</f>
+        <v>1.4202873986992524E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43">
+        <f>B41/B42</f>
+        <v>0.96621832396950269</v>
+      </c>
+      <c r="D43">
+        <f>SQRT((D41/B41)^2+(D42/B42)^2)*B43</f>
+        <v>1.138765092111237E-2</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F43" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="G43" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B38">
-        <f>1-B37</f>
-        <v>3.6801190494080815E-2</v>
-      </c>
-      <c r="D38">
-        <f>D37</f>
-        <v>1.2470816356674488E-2</v>
-      </c>
-      <c r="E38" s="6">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44">
+        <f>1-B43</f>
+        <v>3.378167603049731E-2</v>
+      </c>
+      <c r="D44">
+        <f>D43</f>
+        <v>1.138765092111237E-2</v>
+      </c>
+      <c r="E44" s="6">
         <v>3.8744399999999998E-2</v>
       </c>
-      <c r="F38" s="3">
-        <f>B38-E38</f>
-        <v>-1.9432095059191828E-3</v>
-      </c>
-      <c r="G38" s="7">
-        <f>F38/E38</f>
-        <v>-5.015459023547101E-2</v>
+      <c r="F44" s="3">
+        <f>B44-E44</f>
+        <v>-4.9627239695026887E-3</v>
+      </c>
+      <c r="G44" s="7">
+        <f>F44/E44</f>
+        <v>-0.12808880688570964</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Photometry Time Series Plots
The photometry code now does time series plots and has been cleaned up a lot. The ComputeNetRateJupiter code now does plots of the apertures and annuli.
</commit_message>
<xml_diff>
--- a/Transmission.xlsx
+++ b/Transmission.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02445DDC-A2E2-4463-891A-BCCE1A5B94F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F5044C-46F7-4475-BCBC-21F1D382DAFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35940" yWindow="1830" windowWidth="17520" windowHeight="10800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transmission" sheetId="1" r:id="rId1"/>
@@ -2225,7 +2225,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B14667F8-DBB0-4F95-A6CE-91BC2D82D2A4}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2236,7 +2236,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="13001625" cy="9441656"/>
+    <xdr:ext cx="12981214" cy="9416143"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2562,10 +2562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3362,22 +3362,90 @@
         <v>0.23906510389751026</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="K19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="L20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="M22">
+        <v>1.31053592471522</v>
+      </c>
+      <c r="N22">
+        <v>1.3180147898819501</v>
+      </c>
+      <c r="O22">
+        <v>1.3255149864261599</v>
+      </c>
+      <c r="P22">
+        <v>1.3294236804447499</v>
+      </c>
+      <c r="Q22">
+        <v>1.3193608403941499</v>
+      </c>
+      <c r="R22">
+        <v>1.3021362386437201</v>
+      </c>
+      <c r="S22">
+        <v>1.2633638234167901</v>
+      </c>
+      <c r="T22">
+        <v>1.32281728848747</v>
+      </c>
+      <c r="U22">
+        <v>1.3126421904742001</v>
+      </c>
+      <c r="V22">
+        <v>1.3592245152836699</v>
+      </c>
+      <c r="W22">
+        <v>1.2936623929168301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B23" s="16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M23">
+        <v>1.39026602776317</v>
+      </c>
+      <c r="N23">
+        <v>1.32455698354406</v>
+      </c>
+      <c r="O23">
+        <v>1.3437713149717201</v>
+      </c>
+      <c r="P23">
+        <v>1.37939673924573</v>
+      </c>
+      <c r="Q23">
+        <v>1.33124791614855</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>1.3401078624894101</v>
+      </c>
+      <c r="T23">
+        <v>1.2911119934713799</v>
+      </c>
+      <c r="U23">
+        <v>1.25140575850842</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -3401,8 +3469,41 @@
         <f>D30/D24</f>
         <v>3.8297427069870862</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M24">
+        <v>1.35525957153332</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>1.3838685315935699</v>
+      </c>
+      <c r="P24">
+        <v>1.3591177192686601</v>
+      </c>
+      <c r="Q24">
+        <v>1.3245390271084101</v>
+      </c>
+      <c r="R24">
+        <v>1.3460474924090999</v>
+      </c>
+      <c r="S24">
+        <v>1.3670627471057</v>
+      </c>
+      <c r="T24">
+        <v>1.3645079696737501</v>
+      </c>
+      <c r="U24">
+        <v>1.30242279029534</v>
+      </c>
+      <c r="V24">
+        <v>1.3959268086449499</v>
+      </c>
+      <c r="W24">
+        <v>1.31818328751261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -3426,8 +3527,41 @@
         <f>D31/D25</f>
         <v>1.3604783922106594</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>1.3869868886030301</v>
+      </c>
+      <c r="O25">
+        <v>1.3869598871814099</v>
+      </c>
+      <c r="P25">
+        <v>1.3761891095215999</v>
+      </c>
+      <c r="Q25">
+        <v>1.3309374819703499</v>
+      </c>
+      <c r="R25">
+        <v>1.3822709814534</v>
+      </c>
+      <c r="S25">
+        <v>1.2795650561368701</v>
+      </c>
+      <c r="T25">
+        <v>1.32844339214369</v>
+      </c>
+      <c r="U25">
+        <v>1.2991714499632401</v>
+      </c>
+      <c r="V25">
+        <v>1.3628846375641901</v>
+      </c>
+      <c r="W25">
+        <v>1.2987532518972</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -3448,8 +3582,41 @@
       <c r="G26" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>1.3550637838864401</v>
+      </c>
+      <c r="P26">
+        <v>1.37034046772109</v>
+      </c>
+      <c r="Q26">
+        <v>1.4169305237196099</v>
+      </c>
+      <c r="R26">
+        <v>1.3153442636025801</v>
+      </c>
+      <c r="S26">
+        <v>1.33103154263489</v>
+      </c>
+      <c r="T26">
+        <v>1.3704551496782</v>
+      </c>
+      <c r="U26">
+        <v>1.2917919514534399</v>
+      </c>
+      <c r="V26">
+        <v>1.3596883934483199</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -3473,20 +3640,108 @@
         <v>-0.17492601892449303</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M28">
+        <f>B4/M22-1</f>
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <f t="shared" ref="N28:W28" si="6">C4/N22-1</f>
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="6"/>
+        <v>4.4635740056353512E-4</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B29" s="16" t="s">
         <v>34</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M29">
+        <f t="shared" ref="M29:M32" si="7">B5/M23-1</f>
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ref="N29:N33" si="8">C5/N23-1</f>
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ref="O29:O33" si="9">D5/O23-1</f>
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <f t="shared" ref="P29:P33" si="10">E5/P23-1</f>
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" ref="Q29:Q33" si="11">F5/Q23-1</f>
+        <v>0</v>
+      </c>
+      <c r="R29" t="e">
+        <f t="shared" ref="R29:R33" si="12">G5/R23-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S29">
+        <f t="shared" ref="S29:S33" si="13">H5/S23-1</f>
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <f t="shared" ref="T29:T33" si="14">I5/T23-1</f>
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <f t="shared" ref="U29:U33" si="15">J5/U23-1</f>
+        <v>1.2214438132551741E-2</v>
+      </c>
+      <c r="V29" t="e">
+        <f t="shared" ref="V29:V33" si="16">K5/V23-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W29" t="e">
+        <f t="shared" ref="W29:W32" si="17">L5/W23-1</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -3505,8 +3760,52 @@
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N30" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="15"/>
+        <v>-1.7480050967272343E-3</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -3525,8 +3824,52 @@
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M31" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="15"/>
+        <v>3.0496866050259142E-2</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -3548,6 +3891,50 @@
         <v>28</v>
       </c>
       <c r="H32" s="8"/>
+      <c r="M32" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N32" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="15"/>
+        <v>2.0451761163904569E-2</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W32" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -3862,8 +4249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95EF8F06-C3C6-4CCB-BB0C-8503114DC839}">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>